<commit_message>
updating email use cases
</commit_message>
<xml_diff>
--- a/main/src/offerdiary/doc/workflows.xlsx
+++ b/main/src/offerdiary/doc/workflows.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login-Signup" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="136">
   <si>
     <t>Major Feature</t>
   </si>
@@ -447,6 +447,16 @@
     <t>Add Following objects from session to Globle Object in page - 
 User
 FbAppID</t>
+  </si>
+  <si>
+    <t>All Cards</t>
+  </si>
+  <si>
+    <t>Fix Email framework</t>
+  </si>
+  <si>
+    <t>Extract Common template and message part
+Email Object should get data from callers, params should be constructed inside specific email object</t>
   </si>
 </sst>
 </file>
@@ -1062,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,7 +1235,7 @@
   <dimension ref="B2:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,21 +1308,38 @@
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="F16" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="F18" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>126</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>127</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -1390,6 +1417,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1601,10 +1629,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J33"/>
+  <dimension ref="B2:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1768,9 +1796,20 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="3:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C33" s="2" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>